<commit_message>
Committing new files to repo.
</commit_message>
<xml_diff>
--- a/ED_Gender_2018.xlsx
+++ b/ED_Gender_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hudsonmiller/Desktop/Gov 1005/Final Project/Milestone 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C60EE179-6E87-3C40-8F57-444264B92EAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0C4987-3324-3941-A009-9C6B6CF82C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableLibrary" sheetId="1" r:id="rId1"/>
@@ -30,96 +30,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>All institutions</t>
-  </si>
-  <si>
-    <t>Total_2yr</t>
-  </si>
-  <si>
-    <t>Men_2yr</t>
-  </si>
-  <si>
-    <t>Women_2yr</t>
-  </si>
-  <si>
-    <t>Men_-2yr</t>
-  </si>
-  <si>
-    <t>Women_-2yr</t>
-  </si>
-  <si>
-    <t>Total_-2yr</t>
-  </si>
-  <si>
-    <t>Applications_ALL</t>
-  </si>
-  <si>
-    <t>Admissions_ALL</t>
-  </si>
-  <si>
-    <t>Enrollments_ALL</t>
-  </si>
-  <si>
-    <t>Full-time_ALL</t>
-  </si>
-  <si>
-    <t>Part-time_ALL</t>
-  </si>
-  <si>
-    <t>Applications_Pub</t>
-  </si>
-  <si>
-    <t>Admissions_Pub</t>
-  </si>
-  <si>
-    <t>Enrollments_Pub</t>
-  </si>
-  <si>
-    <t>Full-time_Pub</t>
-  </si>
-  <si>
-    <t>Part-time_Pub</t>
-  </si>
-  <si>
-    <t>Applications_Pvt_NP</t>
-  </si>
-  <si>
-    <t>Admissions_Pvt_NP</t>
-  </si>
-  <si>
-    <t>Enrollments_Pvt_NP</t>
-  </si>
-  <si>
-    <t>Full-time_Pvt_NP</t>
-  </si>
-  <si>
-    <t>Part-time_Pvt_NP</t>
-  </si>
-  <si>
-    <t>Applications_Pvt_FP</t>
-  </si>
-  <si>
-    <t>Admissions_Pvt_FP</t>
-  </si>
-  <si>
-    <t>Enrollments_Pvt_FP</t>
-  </si>
-  <si>
-    <t>Full-time_Pvt_FP</t>
-  </si>
-  <si>
-    <t>Part-time_Pvt_FP</t>
-  </si>
-  <si>
-    <t>Men_4yr</t>
-  </si>
-  <si>
-    <t>Total_4yr</t>
-  </si>
-  <si>
-    <t>Women_4yr</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>Population Group</t>
+  </si>
+  <si>
+    <t>Total Applicants</t>
+  </si>
+  <si>
+    <t>Total Admitted</t>
+  </si>
+  <si>
+    <t>Total Enrollment</t>
+  </si>
+  <si>
+    <t>Total Full Time</t>
+  </si>
+  <si>
+    <t>Total Part Time</t>
+  </si>
+  <si>
+    <t>Applicants (Public University)</t>
+  </si>
+  <si>
+    <t>Enrollment (Public University)</t>
+  </si>
+  <si>
+    <t>Full Time Students (Public University)</t>
+  </si>
+  <si>
+    <t>Part Time Students (Public University)</t>
+  </si>
+  <si>
+    <t>Applicants (Private University)</t>
+  </si>
+  <si>
+    <t>Admitted (Public University)</t>
+  </si>
+  <si>
+    <t>Admitted (Private University)</t>
+  </si>
+  <si>
+    <t>Enrollment (Private University)</t>
+  </si>
+  <si>
+    <t>Full Time Students (Private University)</t>
+  </si>
+  <si>
+    <t>Part Time Students (Private University)</t>
+  </si>
+  <si>
+    <t>Applicant (Private University)</t>
+  </si>
+  <si>
+    <t>Admitted  (Private For Profit University)</t>
+  </si>
+  <si>
+    <t>Enrollment (Private For Profit University)</t>
+  </si>
+  <si>
+    <t>Full Time (Private For Profit University)</t>
+  </si>
+  <si>
+    <t>Part Time (Private For Profit University)</t>
+  </si>
+  <si>
+    <t>All Institutions</t>
+  </si>
+  <si>
+    <t>Total (4 Year)</t>
+  </si>
+  <si>
+    <t>Male (4 Year)</t>
+  </si>
+  <si>
+    <t>Female (4 Year)</t>
+  </si>
+  <si>
+    <t>Total (2 Year)</t>
+  </si>
+  <si>
+    <t>Male (2 Year)</t>
+  </si>
+  <si>
+    <t>Female (2 Year)</t>
+  </si>
+  <si>
+    <t>Total (Less than 2 Year)</t>
+  </si>
+  <si>
+    <t>Female (Less Than 2 Year)</t>
+  </si>
+  <si>
+    <t>Male (Less Than 2 Year)</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,40 +490,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>11284563</v>
@@ -555,7 +561,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>6270275</v>
@@ -590,7 +596,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1629162</v>
@@ -625,7 +631,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1579537</v>
@@ -660,7 +666,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>49625</v>
@@ -695,7 +701,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>6355793</v>
@@ -730,7 +736,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>3809157</v>
@@ -765,7 +771,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1092348</v>
@@ -800,7 +806,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1059517</v>
@@ -835,7 +841,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>32831</v>
@@ -870,7 +876,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>4834855</v>
@@ -905,7 +911,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>2395320</v>
@@ -940,7 +946,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>514858</v>
@@ -975,7 +981,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>501103</v>
@@ -1010,7 +1016,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>13755</v>
@@ -1045,7 +1051,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>93915</v>
@@ -1080,7 +1086,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>65798</v>
@@ -1115,7 +1121,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>21956</v>
@@ -1150,7 +1156,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>18917</v>
@@ -1185,7 +1191,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>3039</v>

</xml_diff>